<commit_message>
Added Excel Utility using Apache POI 5
</commit_message>
<xml_diff>
--- a/src/main/resources/Testdata.xlsx
+++ b/src/main/resources/Testdata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,9 +15,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Password_FromExcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid userName
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid password
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    UserName_FromExcel</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +44,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -42,18 +74,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +435,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>